<commit_message>
Update the tensorflow code.
</commit_message>
<xml_diff>
--- a/kpi/ZL_2019 DQA Weekly Report.xlsx
+++ b/kpi/ZL_2019 DQA Weekly Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="1230" windowWidth="19395" windowHeight="7335" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="375" yWindow="1230" windowWidth="19395" windowHeight="7335" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sample" sheetId="1" r:id="rId1"/>
@@ -11412,6 +11412,846 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">A. Ongoing Project
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+B. Planning Project
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- none</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+C. Report
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+D. Meeting
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- none</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+E. Other</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Auto Installation by PXE Server static ip address.
+- Tensorflow Operation of GPU speed up.
+- ProgrammingIndex by PyQT.
+- Mechanical arm AutoIT method.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A. Ongoing Project
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+B. Planning Project
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- none</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+C. Report
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+D. Meeting
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- none</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+E. Other</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Android 8.1 for WLAN ans WWAN of airplane mode
+- Auto Installation by PXE Server static ip address.
+- Tensorflow Operation of GPU speed up.
+- ProgrammingIndex by PyQT.
+- Mechanical arm AutoIT method.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A. Ongoing Project
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+B. Planning Project
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- none</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+C. Report
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+D. Meeting
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- none</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+E. Other
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Android 8.1 for WLAN ans WWAN of airplane mode
+- Auto Installation by PXE Server static ip address.
+- Tensorflow Operation of GPU speed up.
+- ProgrammingIndex by PyQT.
+- Mechanical arm AutoIT method.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/11/04~2019/11/08</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/11/11~2019/11/15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/11/18~2019/11/22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/11/25~2019/11/29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">A. Finished
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- none</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+B. Ongoing Project
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">C. Report
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">D. Meeting
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E. Other</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- none</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A. Ongoing Project
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+B. Planning Project
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- none</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+C. Report
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+D. Meeting
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- none</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+E. Other</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- none</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">A. Finished
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- none</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+B. Ongoing Project
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">C. Report
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">D. Meeting
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>E. Other</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Implement the wlan of ethernet and wwan of multi airplane base on Android 8.1. (10/28)
+- Implement the wlan of ethernet and wwan of multi airplane base on Android 8.1. (10/29)
+- Research the Tensorflow Operation of GPU speed up. (10/30~11/01)
+- Anaconda the visual space by the tensorflw-gpu and python 3.5.0 edition. (10/30)
+- Resolved the NVIDIA graphics driver installation error. (10/31)
+- Installation the CUDA 8.0 problem. (11/01)
+- Discusstion the CUDA 8.0 and Geforce GTX 1600 display card error. (11/01)
+- Discusstion the ROCm for AMD GPU performance. (10/31~11/01)</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <rPr>
         <b/>
         <sz val="12"/>
@@ -11576,843 +12416,8 @@
 - Implement the sop of the PXE's Legacy base on x64 execution testing process. (10/22)
 - Implement the sop of the PXE's environment setting by auto testing parameter of xml files. (10/23)
 - Merge the pxe folder and xml file to git server and mantain the test process. (10/23)
-- Implement the wlan of ethernet and wlan of single airplane. (10/24)
-- Implement the wlan of ethernet and wlan of single airplane. (10/25)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A. Ongoing Project
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-B. Planning Project
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- none</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-C. Report
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-D. Meeting
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- none</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-E. Other</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Auto Installation by PXE Server static ip address.
-- Tensorflow Operation of GPU speed up.
-- ProgrammingIndex by PyQT.
-- Mechanical arm AutoIT method.</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A. Ongoing Project
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-B. Planning Project
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- none</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-C. Report
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-D. Meeting
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- none</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-E. Other</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Android 8.1 for WLAN ans WWAN of airplane mode
-- Auto Installation by PXE Server static ip address.
-- Tensorflow Operation of GPU speed up.
-- ProgrammingIndex by PyQT.
-- Mechanical arm AutoIT method.</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A. Ongoing Project
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-B. Planning Project
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- none</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-C. Report
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-D. Meeting
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- none</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-E. Other
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Android 8.1 for WLAN ans WWAN of airplane mode
-- Auto Installation by PXE Server static ip address.
-- Tensorflow Operation of GPU speed up.
-- ProgrammingIndex by PyQT.
-- Mechanical arm AutoIT method.</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019/11/04~2019/11/08</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019/11/11~2019/11/15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019/11/18~2019/11/22</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019/11/25~2019/11/29</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">A. Finished
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- none</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-B. Ongoing Project
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">C. Report
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">D. Meeting
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E. Other</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- none</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A. Ongoing Project
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-B. Planning Project
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- none</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-C. Report
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-D. Meeting
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- none</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-E. Other</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- none</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">A. Finished
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- none</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-B. Ongoing Project
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">C. Report
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">D. Meeting
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">none
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>E. Other</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="新細明體"/>
-        <family val="1"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- Implement the wlan of ethernet and wwan of multi airplane. (10/28)
-- Implement the wlan of ethernet and wwan of multi airplane. (10/29)
-- Research the Tensorflow Operation of GPU speed up. (10/30~11/01)</t>
+- Implement the wlan of ethernet and wlan of single airplane base on Android 8.1. (10/24)
+- Implement the wlan of ethernet and wlan of single airplane base on Android 8.1. (10/25)</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -13096,7 +13101,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13174,10 +13181,10 @@
         <v>132</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -13186,10 +13193,10 @@
         <v>131</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -13204,7 +13211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -13241,10 +13248,10 @@
     </row>
     <row r="3" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>152</v>
@@ -13253,37 +13260,37 @@
     </row>
     <row r="4" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="D6" s="1"/>
     </row>

</xml_diff>

<commit_message>
Update the kpi folder
</commit_message>
<xml_diff>
--- a/kpi/ZL_2019 DQA Weekly Report.xlsx
+++ b/kpi/ZL_2019 DQA Weekly Report.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="158">
   <si>
     <t>Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -12905,6 +12905,132 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">A. Ongoing Project
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+B. Planning Project
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- none</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+C. Report
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- none
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+D. Meeting
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- none</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+E. Other</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="新細明體"/>
+        <family val="1"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Auto Installation by PXE Server static ip address.
+- ProgrammingIndex by PyQT.
+- PassMark for BurnInTest for the quicktest.
+- Mechanical arm AutoIT method.
+- CI Sourcing.
+- Prepare the test automation report for Q1.
+- Airplane on/off for windows of other resolution.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <rPr>
         <b/>
         <sz val="12"/>
@@ -13062,7 +13188,11 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-- none</t>
+- Coding the timer read and writing base on application and operation log. (11/25~11/26)
+- Implement the three pxe server build. (11/27)
+- Airplane for windows resolution. (11/28)
+- BurnInTest USB AutoRun. (11/29)
+- ProgramIndex Design. (11/29)</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -13691,7 +13821,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13767,10 +13899,10 @@
         <v>146</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D6" s="1"/>
     </row>

</xml_diff>

<commit_message>
Commit the weekly report.
</commit_message>
<xml_diff>
--- a/kpi/ZL_2019 DQA Weekly Report.xlsx
+++ b/kpi/ZL_2019 DQA Weekly Report.xlsx
@@ -13190,10 +13190,12 @@
       <t xml:space="preserve">
 - Coding the timer read and writing base on application and operation log. (11/25~11/26)
 - Finished the WDS other DUT system environment setting. (11/26)
+- Setting the ubuntu OS base on window system. (11/27~11/28)
 - Implement the three pxe server build. (11/27)
 - Airplane for windows resolution. (11/28)
-- BurnInTest USB AutoRun. (11/29)
-- ProgramIndex Design. (11/29)</t>
+- Continuou intergration base on Ubuntu 18.04 environment setting. (11/28)
+- Study the BurnInTest USB AutoRun documnet. (11/29)
+- ProgramIndex Design by PyQT User interface. (11/29)</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -13822,9 +13824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>